<commit_message>
Updating core Branch with new tests
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/ContactPage.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/ContactPage.xlsx
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Automate remaining test cases
1. Test Cases for Download Get Started
2. Test Cases for Download Start Today
3. Test Cases forProfessional service page
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/ContactPage.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/ContactPage.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/LocatorDictionary/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF790E1-918F-714D-AD3C-C810C35259FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19140" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
@@ -178,19 +184,19 @@
     <t>ContactPage_CheckBox_PrivacyConsent</t>
   </si>
   <si>
-    <t>input#mktoCheckbox_142098_0</t>
-  </si>
-  <si>
     <t>ContactPage_Label_PrivacyConsent</t>
   </si>
   <si>
-    <t>label#LblmktoCheckbox_142098_0</t>
+    <t>div.mktoCheckboxList input</t>
+  </si>
+  <si>
+    <t>div.mktoCheckboxList label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,14 +248,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -287,7 +296,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -359,7 +368,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -532,20 +541,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="64.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -567,7 +576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,7 +587,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -589,7 +598,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -600,7 +609,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -611,7 +620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -622,7 +631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -633,7 +642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -644,7 +653,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -655,7 +664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -666,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -677,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -688,7 +697,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -699,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -710,7 +719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -721,7 +730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -732,7 +741,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -743,7 +752,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -754,7 +763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -765,7 +774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -776,7 +785,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -787,7 +796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -798,7 +807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -809,7 +818,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -820,7 +829,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -831,7 +840,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -839,22 +848,22 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C12">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>